<commit_message>
Contact case Test scripts
</commit_message>
<xml_diff>
--- a/SDET_11/src/test/resources/data/Input Data.xlsx
+++ b/SDET_11/src/test/resources/data/Input Data.xlsx
@@ -4,19 +4,19 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16515" windowHeight="2745"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="14805" windowHeight="3375" activeTab="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="Account" sheetId="2" r:id="rId2"/>
+    <sheet name="Account" sheetId="2" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId2"/>
   </sheets>
   <calcPr calcId="0"/>
-  <oleSize ref="A1:P7"/>
+  <oleSize ref="A1:N9"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="41">
   <si>
     <t>Hai hello how r u</t>
   </si>
@@ -79,19 +79,92 @@
   </si>
   <si>
     <t>QSPHYD3</t>
+  </si>
+  <si>
+    <t>Team Leader</t>
+  </si>
+  <si>
+    <t>IT</t>
+  </si>
+  <si>
+    <t>sureshabc@gmail.com</t>
+  </si>
+  <si>
+    <t>Mrs.</t>
+  </si>
+  <si>
+    <t>Chandana</t>
+  </si>
+  <si>
+    <t>chandanaabc@gmail.com</t>
+  </si>
+  <si>
+    <t>setty</t>
+  </si>
+  <si>
+    <t>Raju</t>
+  </si>
+  <si>
+    <t>Partner</t>
+  </si>
+  <si>
+    <t>Dr.</t>
+  </si>
+  <si>
+    <t>Pramod</t>
+  </si>
+  <si>
+    <t>Conference</t>
+  </si>
+  <si>
+    <t>13235551234@efaxsend.com</t>
+  </si>
+  <si>
+    <t>Tiger crm is used to store all the types of data of different customers</t>
+  </si>
+  <si>
+    <t>Prof.</t>
+  </si>
+  <si>
+    <t>Ranjan</t>
+  </si>
+  <si>
+    <t>Singala</t>
+  </si>
+  <si>
+    <t>Word of mouth</t>
+  </si>
+  <si>
+    <t>KPHB Phase 1</t>
+  </si>
+  <si>
+    <t>India</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color rgb="FF202124"/>
+      <name val="Consolas"/>
+      <family val="3"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color rgb="FF202124"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -114,9 +187,16 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -421,62 +501,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G2"/>
-  <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F5" sqref="F5"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="3" max="3" width="11" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A2" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="C2" s="1">
-        <v>6281963899</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -678,4 +706,147 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:I6"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F6" sqref="F6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="3" max="3" width="11" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.5703125" customWidth="1"/>
+    <col min="5" max="5" width="17.140625" customWidth="1"/>
+    <col min="6" max="6" width="19.140625" customWidth="1"/>
+    <col min="7" max="7" width="23.85546875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="F1" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" ht="24" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C2" s="1">
+        <v>6281963899</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="E2" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="G2" s="4" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="D3" s="1">
+        <v>123456789</v>
+      </c>
+      <c r="E3" s="4" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="C4" s="1">
+        <v>8976523104</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" ht="48" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="D5" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="E5" s="4" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A6" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="E6" s="1">
+        <v>8978523134</v>
+      </c>
+      <c r="F6" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="G6" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="H6" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="I6" s="1" t="s">
+        <v>40</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>